<commit_message>
Updated to include an approx
</commit_message>
<xml_diff>
--- a/Lab work/Materials lab/Charpy and Hardness Data 2025.xlsx
+++ b/Lab work/Materials lab/Charpy and Hardness Data 2025.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/eb1723_ic_ac_uk/Documents/ME2/University computing/Lab work/Materials lab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{1539A9E4-AFA8-425B-AFF2-01C484C56F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36DE12E4-7E73-A949-B69E-12BA5C629B5C}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="8_{1539A9E4-AFA8-425B-AFF2-01C484C56F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{97C0A14E-FACD-47A3-BA63-7AE97CB9C5E3}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{81260FE9-10E2-42F8-90B5-15DA67BC97B4}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{81260FE9-10E2-42F8-90B5-15DA67BC97B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hardness Data" sheetId="6" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Aluminium" sheetId="4" r:id="rId5"/>
     <sheet name="Zinc" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -177,6 +177,1057 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Hardness against 1/(√D) where D is grain diameter </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Hardness Data'!$AA$3:$AA$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>7.905694150420949</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99209473766568124</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.7042952122737639</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Hardness Data'!$V$3:$V$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>193.65500000000003</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>121.66500000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>119.83</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3BCF-4B66-8AEC-F62BAAC61857}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="41286063"/>
+        <c:axId val="41287023"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="41286063"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>1/</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>√D</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="41287023"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="41287023"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Hardness by HV10/</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="41286063"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>82826</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>24019</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>588065</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>33958</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8825923A-F828-58A3-15EC-F22ECDA8ED10}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -496,19 +1547,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1F2B471-7B7B-4EF9-BA2C-36EAA62002E6}">
-  <dimension ref="A2:U16"/>
+  <dimension ref="A2:AA16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AA3" sqref="AA3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" customWidth="1"/>
-    <col min="2" max="21" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.125" customWidth="1"/>
+    <col min="2" max="21" width="5.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:21" ht="18" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:27" ht="18.75" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
@@ -570,7 +1621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -634,168 +1685,238 @@
       <c r="U3" s="3">
         <v>191.2</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="V3" s="4">
+        <f>SUM(B3:U3)/20</f>
+        <v>193.65500000000003</v>
+      </c>
+      <c r="W3" s="4">
+        <f>MAX(B3:U3)</f>
+        <v>200.3</v>
+      </c>
+      <c r="X3" s="4">
+        <f>MIN(B3:U3)</f>
+        <v>188.5</v>
+      </c>
+      <c r="Y3">
+        <f>(W3-X3)/19</f>
+        <v>0.62105263157894797</v>
+      </c>
+      <c r="Z3">
+        <v>1.6E-2</v>
+      </c>
+      <c r="AA3">
+        <f>1/SQRT(Z3)</f>
+        <v>7.905694150420949</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>120.8</v>
+      </c>
+      <c r="C4" s="3">
+        <v>121.7</v>
+      </c>
+      <c r="D4" s="3">
+        <v>125.3</v>
+      </c>
+      <c r="E4" s="3">
+        <v>123.4</v>
+      </c>
+      <c r="F4" s="3">
+        <v>120.7</v>
+      </c>
+      <c r="G4" s="3">
+        <v>122.6</v>
+      </c>
+      <c r="H4" s="3">
+        <v>119</v>
+      </c>
+      <c r="I4" s="3">
+        <v>116.4</v>
+      </c>
+      <c r="J4" s="3">
+        <v>119</v>
+      </c>
+      <c r="K4" s="3">
+        <v>122.2</v>
+      </c>
+      <c r="L4" s="3">
+        <v>122.5</v>
+      </c>
+      <c r="M4" s="3">
+        <v>124.7</v>
+      </c>
+      <c r="N4" s="3">
+        <v>128.69999999999999</v>
+      </c>
+      <c r="O4" s="3">
+        <v>125.4</v>
+      </c>
+      <c r="P4" s="3">
+        <v>121.7</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>122.7</v>
+      </c>
+      <c r="R4" s="3">
+        <v>119.5</v>
+      </c>
+      <c r="S4" s="3">
+        <v>117.8</v>
+      </c>
+      <c r="T4" s="3">
+        <v>120.9</v>
+      </c>
+      <c r="U4" s="3">
+        <v>118.3</v>
+      </c>
+      <c r="V4" s="4">
+        <f t="shared" ref="V4:V5" si="0">SUM(B4:U4)/20</f>
+        <v>121.66500000000003</v>
+      </c>
+      <c r="W4" s="4">
+        <f t="shared" ref="W4:W5" si="1">MAX(B4:U4)</f>
+        <v>128.69999999999999</v>
+      </c>
+      <c r="X4" s="4">
+        <f t="shared" ref="X4:X5" si="2">MIN(B4:U4)</f>
+        <v>116.4</v>
+      </c>
+      <c r="Y4">
+        <f t="shared" ref="Y4:Y5" si="3">(W4-X4)/19</f>
+        <v>0.6473684210526307</v>
+      </c>
+      <c r="Z4">
+        <v>1.016</v>
+      </c>
+      <c r="AA4">
+        <f t="shared" ref="AA4:AA5" si="4">1/SQRT(Z4)</f>
+        <v>0.99209473766568124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B5" s="3">
         <v>116.1</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C5" s="3">
         <v>116.1</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D5" s="3">
         <v>118.3</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E5" s="3">
         <v>118.5</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F5" s="3">
         <v>122.4</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G5" s="3">
         <v>122.1</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H5" s="3">
         <v>116.9</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I5" s="3">
         <v>113.9</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J5" s="3">
         <v>117</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K5" s="3">
         <v>108.7</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L5" s="3">
         <v>115.1</v>
       </c>
-      <c r="M4" s="3">
+      <c r="M5" s="3">
         <v>120.5</v>
       </c>
-      <c r="N4" s="3">
+      <c r="N5" s="3">
         <v>124.6</v>
       </c>
-      <c r="O4" s="3">
+      <c r="O5" s="3">
         <v>125.3</v>
       </c>
-      <c r="P4" s="3">
+      <c r="P5" s="3">
         <v>120.8</v>
       </c>
-      <c r="Q4" s="3">
+      <c r="Q5" s="3">
         <v>124</v>
       </c>
-      <c r="R4" s="3">
+      <c r="R5" s="3">
         <v>129.69999999999999</v>
       </c>
-      <c r="S4" s="3">
+      <c r="S5" s="3">
         <v>120.9</v>
       </c>
-      <c r="T4" s="3">
+      <c r="T5" s="3">
         <v>119.4</v>
       </c>
-      <c r="U4" s="3">
+      <c r="U5" s="3">
         <v>126.3</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3">
-        <v>120.8</v>
-      </c>
-      <c r="C5" s="3">
-        <v>121.7</v>
-      </c>
-      <c r="D5" s="3">
-        <v>125.3</v>
-      </c>
-      <c r="E5" s="3">
-        <v>123.4</v>
-      </c>
-      <c r="F5" s="3">
-        <v>120.7</v>
-      </c>
-      <c r="G5" s="3">
-        <v>122.6</v>
-      </c>
-      <c r="H5" s="3">
-        <v>119</v>
-      </c>
-      <c r="I5" s="3">
-        <v>116.4</v>
-      </c>
-      <c r="J5" s="3">
-        <v>119</v>
-      </c>
-      <c r="K5" s="3">
-        <v>122.2</v>
-      </c>
-      <c r="L5" s="3">
-        <v>122.5</v>
-      </c>
-      <c r="M5" s="3">
-        <v>124.7</v>
-      </c>
-      <c r="N5" s="3">
-        <v>128.69999999999999</v>
-      </c>
-      <c r="O5" s="3">
-        <v>125.4</v>
-      </c>
-      <c r="P5" s="3">
-        <v>121.7</v>
-      </c>
-      <c r="Q5" s="3">
-        <v>122.7</v>
-      </c>
-      <c r="R5" s="3">
-        <v>119.5</v>
-      </c>
-      <c r="S5" s="3">
-        <v>117.8</v>
-      </c>
-      <c r="T5" s="3">
-        <v>120.9</v>
-      </c>
-      <c r="U5" s="3">
-        <v>118.3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="V5" s="4">
+        <f t="shared" si="0"/>
+        <v>119.83</v>
+      </c>
+      <c r="W5" s="4">
+        <f t="shared" si="1"/>
+        <v>129.69999999999999</v>
+      </c>
+      <c r="X5" s="4">
+        <f t="shared" si="2"/>
+        <v>108.7</v>
+      </c>
+      <c r="Y5">
+        <f t="shared" si="3"/>
+        <v>1.1052631578947361</v>
+      </c>
+      <c r="Z5">
+        <v>2.016</v>
+      </c>
+      <c r="AA5">
+        <f t="shared" si="4"/>
+        <v>0.7042952122737639</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="I9" s="4"/>
       <c r="L9" s="4"/>
       <c r="P9" s="6"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="I10" s="4"/>
       <c r="J10" s="5"/>
       <c r="L10" s="4"/>
       <c r="P10" s="6"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="I11" s="4"/>
       <c r="L11" s="4"/>
       <c r="P11" s="6"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="I14" s="4"/>
       <c r="L14" s="4"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="I15" s="4"/>
       <c r="L15" s="4"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="I16" s="4"/>
       <c r="L16" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -803,17 +1924,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD1DA1BD-F8F6-475A-98D3-9778393B6783}">
   <dimension ref="A1:B73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -821,7 +1942,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>200</v>
       </c>
@@ -829,7 +1950,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>200</v>
       </c>
@@ -837,7 +1958,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>200</v>
       </c>
@@ -845,7 +1966,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>200</v>
       </c>
@@ -853,7 +1974,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>200</v>
       </c>
@@ -861,7 +1982,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>200</v>
       </c>
@@ -869,7 +1990,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>100</v>
       </c>
@@ -877,7 +1998,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>100</v>
       </c>
@@ -885,7 +2006,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>100</v>
       </c>
@@ -893,7 +2014,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>100</v>
       </c>
@@ -901,7 +2022,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>100</v>
       </c>
@@ -909,7 +2030,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>100</v>
       </c>
@@ -917,7 +2038,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>100</v>
       </c>
@@ -925,7 +2046,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>100</v>
       </c>
@@ -933,7 +2054,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>100</v>
       </c>
@@ -941,7 +2062,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>80</v>
       </c>
@@ -949,7 +2070,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>70</v>
       </c>
@@ -957,7 +2078,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>50</v>
       </c>
@@ -965,7 +2086,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>50</v>
       </c>
@@ -973,7 +2094,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>50</v>
       </c>
@@ -981,7 +2102,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>50</v>
       </c>
@@ -989,7 +2110,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>50</v>
       </c>
@@ -997,7 +2118,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>50</v>
       </c>
@@ -1005,7 +2126,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>50</v>
       </c>
@@ -1013,7 +2134,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>20</v>
       </c>
@@ -1021,7 +2142,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>20</v>
       </c>
@@ -1029,7 +2150,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>20</v>
       </c>
@@ -1037,7 +2158,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>20</v>
       </c>
@@ -1045,7 +2166,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>20</v>
       </c>
@@ -1053,7 +2174,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>20</v>
       </c>
@@ -1061,7 +2182,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>20</v>
       </c>
@@ -1069,7 +2190,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>20</v>
       </c>
@@ -1077,7 +2198,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>20</v>
       </c>
@@ -1085,7 +2206,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>0</v>
       </c>
@@ -1093,7 +2214,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>0</v>
       </c>
@@ -1101,7 +2222,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>0</v>
       </c>
@@ -1109,7 +2230,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>0</v>
       </c>
@@ -1117,7 +2238,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>0</v>
       </c>
@@ -1125,7 +2246,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>0</v>
       </c>
@@ -1133,7 +2254,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>0</v>
       </c>
@@ -1141,7 +2262,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>0</v>
       </c>
@@ -1149,7 +2270,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>0</v>
       </c>
@@ -1157,7 +2278,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>-20</v>
       </c>
@@ -1165,7 +2286,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>-20</v>
       </c>
@@ -1173,7 +2294,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>-20</v>
       </c>
@@ -1181,7 +2302,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>-20</v>
       </c>
@@ -1189,7 +2310,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>-20</v>
       </c>
@@ -1197,7 +2318,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>-20</v>
       </c>
@@ -1205,7 +2326,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>-20</v>
       </c>
@@ -1213,7 +2334,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>-20</v>
       </c>
@@ -1221,7 +2342,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>-20</v>
       </c>
@@ -1229,7 +2350,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>-50</v>
       </c>
@@ -1237,7 +2358,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>-50</v>
       </c>
@@ -1245,7 +2366,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>-50</v>
       </c>
@@ -1253,7 +2374,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>-50</v>
       </c>
@@ -1261,7 +2382,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>-50</v>
       </c>
@@ -1269,7 +2390,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>-50</v>
       </c>
@@ -1277,7 +2398,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>-80</v>
       </c>
@@ -1285,7 +2406,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>-80</v>
       </c>
@@ -1293,7 +2414,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>-80</v>
       </c>
@@ -1301,7 +2422,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>-80</v>
       </c>
@@ -1309,7 +2430,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>-80</v>
       </c>
@@ -1317,7 +2438,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>-80</v>
       </c>
@@ -1325,7 +2446,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>-80</v>
       </c>
@@ -1333,7 +2454,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>-80</v>
       </c>
@@ -1341,7 +2462,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>-80</v>
       </c>
@@ -1349,7 +2470,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>-195</v>
       </c>
@@ -1357,7 +2478,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>-195</v>
       </c>
@@ -1365,7 +2486,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>-195</v>
       </c>
@@ -1373,7 +2494,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>-195</v>
       </c>
@@ -1381,7 +2502,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>-195</v>
       </c>
@@ -1389,7 +2510,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>-195</v>
       </c>
@@ -1410,13 +2531,13 @@
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -1424,7 +2545,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>200</v>
       </c>
@@ -1432,7 +2553,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>200</v>
       </c>
@@ -1440,7 +2561,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>200</v>
       </c>
@@ -1448,7 +2569,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>200</v>
       </c>
@@ -1456,7 +2577,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>200</v>
       </c>
@@ -1464,7 +2585,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>200</v>
       </c>
@@ -1472,7 +2593,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>100</v>
       </c>
@@ -1480,7 +2601,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>100</v>
       </c>
@@ -1488,7 +2609,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>100</v>
       </c>
@@ -1496,7 +2617,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>100</v>
       </c>
@@ -1504,7 +2625,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>100</v>
       </c>
@@ -1512,7 +2633,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>100</v>
       </c>
@@ -1520,7 +2641,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>100</v>
       </c>
@@ -1528,7 +2649,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>100</v>
       </c>
@@ -1536,7 +2657,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>80</v>
       </c>
@@ -1544,7 +2665,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>70</v>
       </c>
@@ -1552,7 +2673,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>50</v>
       </c>
@@ -1560,7 +2681,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>50</v>
       </c>
@@ -1568,7 +2689,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>50</v>
       </c>
@@ -1576,7 +2697,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>50</v>
       </c>
@@ -1584,7 +2705,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>50</v>
       </c>
@@ -1592,7 +2713,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>50</v>
       </c>
@@ -1600,7 +2721,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>20</v>
       </c>
@@ -1608,7 +2729,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>20</v>
       </c>
@@ -1616,7 +2737,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>20</v>
       </c>
@@ -1624,7 +2745,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>20</v>
       </c>
@@ -1632,7 +2753,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>20</v>
       </c>
@@ -1640,7 +2761,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>20</v>
       </c>
@@ -1648,7 +2769,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>20</v>
       </c>
@@ -1656,7 +2777,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>20</v>
       </c>
@@ -1664,7 +2785,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>20</v>
       </c>
@@ -1672,7 +2793,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>0</v>
       </c>
@@ -1680,7 +2801,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>0</v>
       </c>
@@ -1688,7 +2809,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>0</v>
       </c>
@@ -1696,7 +2817,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>0</v>
       </c>
@@ -1704,7 +2825,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>0</v>
       </c>
@@ -1712,7 +2833,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>0</v>
       </c>
@@ -1720,7 +2841,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>0</v>
       </c>
@@ -1728,7 +2849,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>0</v>
       </c>
@@ -1736,7 +2857,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>0</v>
       </c>
@@ -1744,7 +2865,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>-20</v>
       </c>
@@ -1752,7 +2873,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>-20</v>
       </c>
@@ -1760,7 +2881,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>-20</v>
       </c>
@@ -1768,7 +2889,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>-20</v>
       </c>
@@ -1776,7 +2897,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>-20</v>
       </c>
@@ -1784,7 +2905,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>-20</v>
       </c>
@@ -1792,7 +2913,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>-20</v>
       </c>
@@ -1800,7 +2921,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>-20</v>
       </c>
@@ -1808,7 +2929,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>-20</v>
       </c>
@@ -1816,7 +2937,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>-50</v>
       </c>
@@ -1824,7 +2945,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>-50</v>
       </c>
@@ -1832,7 +2953,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>-50</v>
       </c>
@@ -1840,7 +2961,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>-50</v>
       </c>
@@ -1848,7 +2969,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>-50</v>
       </c>
@@ -1856,7 +2977,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>-50</v>
       </c>
@@ -1864,7 +2985,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>-80</v>
       </c>
@@ -1872,7 +2993,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>-80</v>
       </c>
@@ -1880,7 +3001,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>-80</v>
       </c>
@@ -1888,7 +3009,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>-80</v>
       </c>
@@ -1896,7 +3017,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>-80</v>
       </c>
@@ -1904,7 +3025,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>-80</v>
       </c>
@@ -1912,7 +3033,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>-80</v>
       </c>
@@ -1920,7 +3041,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>-80</v>
       </c>
@@ -1928,7 +3049,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>-80</v>
       </c>
@@ -1936,7 +3057,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>-195</v>
       </c>
@@ -1944,7 +3065,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>-195</v>
       </c>
@@ -1952,7 +3073,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>-195</v>
       </c>
@@ -1960,7 +3081,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>-195</v>
       </c>
@@ -1968,7 +3089,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>-195</v>
       </c>
@@ -1976,7 +3097,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>-195</v>
       </c>
@@ -1997,13 +3118,13 @@
       <selection activeCell="A2" sqref="A2:B71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2011,7 +3132,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>200</v>
       </c>
@@ -2019,7 +3140,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>200</v>
       </c>
@@ -2027,7 +3148,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>200</v>
       </c>
@@ -2035,7 +3156,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>200</v>
       </c>
@@ -2043,7 +3164,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>200</v>
       </c>
@@ -2051,7 +3172,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>200</v>
       </c>
@@ -2059,7 +3180,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>100</v>
       </c>
@@ -2067,7 +3188,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>100</v>
       </c>
@@ -2075,7 +3196,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>100</v>
       </c>
@@ -2083,7 +3204,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>100</v>
       </c>
@@ -2091,7 +3212,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>100</v>
       </c>
@@ -2099,7 +3220,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>100</v>
       </c>
@@ -2107,7 +3228,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>100</v>
       </c>
@@ -2115,7 +3236,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>100</v>
       </c>
@@ -2123,7 +3244,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>90</v>
       </c>
@@ -2131,7 +3252,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>70</v>
       </c>
@@ -2139,7 +3260,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>50</v>
       </c>
@@ -2147,7 +3268,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>50</v>
       </c>
@@ -2155,7 +3276,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>50</v>
       </c>
@@ -2163,7 +3284,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>50</v>
       </c>
@@ -2171,7 +3292,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>50</v>
       </c>
@@ -2179,7 +3300,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>50</v>
       </c>
@@ -2187,7 +3308,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>20</v>
       </c>
@@ -2195,7 +3316,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>20</v>
       </c>
@@ -2203,7 +3324,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>20</v>
       </c>
@@ -2211,7 +3332,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>20</v>
       </c>
@@ -2219,7 +3340,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>20</v>
       </c>
@@ -2227,7 +3348,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>20</v>
       </c>
@@ -2235,7 +3356,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>20</v>
       </c>
@@ -2243,7 +3364,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>20</v>
       </c>
@@ -2251,7 +3372,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>20</v>
       </c>
@@ -2259,7 +3380,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>0</v>
       </c>
@@ -2267,7 +3388,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>0</v>
       </c>
@@ -2275,7 +3396,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>0</v>
       </c>
@@ -2283,7 +3404,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>0</v>
       </c>
@@ -2291,7 +3412,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>0</v>
       </c>
@@ -2299,7 +3420,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>0</v>
       </c>
@@ -2307,7 +3428,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>0</v>
       </c>
@@ -2315,7 +3436,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>0</v>
       </c>
@@ -2323,7 +3444,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>0</v>
       </c>
@@ -2331,7 +3452,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>-20</v>
       </c>
@@ -2339,7 +3460,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>-20</v>
       </c>
@@ -2347,7 +3468,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>-20</v>
       </c>
@@ -2355,7 +3476,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>-20</v>
       </c>
@@ -2363,7 +3484,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>-20</v>
       </c>
@@ -2371,7 +3492,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>-20</v>
       </c>
@@ -2379,7 +3500,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>-20</v>
       </c>
@@ -2387,7 +3508,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>-20</v>
       </c>
@@ -2395,7 +3516,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>-20</v>
       </c>
@@ -2403,7 +3524,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>-50</v>
       </c>
@@ -2411,7 +3532,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>-50</v>
       </c>
@@ -2419,7 +3540,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>-50</v>
       </c>
@@ -2427,7 +3548,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>-50</v>
       </c>
@@ -2435,7 +3556,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>-50</v>
       </c>
@@ -2443,7 +3564,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>-50</v>
       </c>
@@ -2451,7 +3572,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>-80</v>
       </c>
@@ -2459,7 +3580,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>-80</v>
       </c>
@@ -2467,7 +3588,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>-80</v>
       </c>
@@ -2475,7 +3596,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>-80</v>
       </c>
@@ -2483,7 +3604,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>-80</v>
       </c>
@@ -2491,7 +3612,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>-80</v>
       </c>
@@ -2499,7 +3620,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>-80</v>
       </c>
@@ -2507,7 +3628,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>-80</v>
       </c>
@@ -2515,7 +3636,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>-80</v>
       </c>
@@ -2523,7 +3644,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>-195</v>
       </c>
@@ -2531,7 +3652,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>-195</v>
       </c>
@@ -2539,7 +3660,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>-195</v>
       </c>
@@ -2547,7 +3668,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>-195</v>
       </c>
@@ -2555,7 +3676,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>-195</v>
       </c>
@@ -2563,7 +3684,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>-195</v>
       </c>
@@ -2584,13 +3705,13 @@
       <selection activeCell="A2" sqref="A2:B73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -2598,7 +3719,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>200</v>
       </c>
@@ -2606,7 +3727,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>200</v>
       </c>
@@ -2614,7 +3735,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>200</v>
       </c>
@@ -2622,7 +3743,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>200</v>
       </c>
@@ -2630,7 +3751,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>200</v>
       </c>
@@ -2638,7 +3759,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>200</v>
       </c>
@@ -2646,7 +3767,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>100</v>
       </c>
@@ -2654,7 +3775,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>100</v>
       </c>
@@ -2662,7 +3783,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>100</v>
       </c>
@@ -2670,7 +3791,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>100</v>
       </c>
@@ -2678,7 +3799,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>100</v>
       </c>
@@ -2686,7 +3807,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>100</v>
       </c>
@@ -2694,7 +3815,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>100</v>
       </c>
@@ -2702,7 +3823,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>100</v>
       </c>
@@ -2710,7 +3831,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>100</v>
       </c>
@@ -2718,7 +3839,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>80</v>
       </c>
@@ -2726,7 +3847,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>70</v>
       </c>
@@ -2734,7 +3855,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>50</v>
       </c>
@@ -2742,7 +3863,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>50</v>
       </c>
@@ -2750,7 +3871,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>50</v>
       </c>
@@ -2758,7 +3879,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>50</v>
       </c>
@@ -2766,7 +3887,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>50</v>
       </c>
@@ -2774,7 +3895,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>50</v>
       </c>
@@ -2782,7 +3903,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>50</v>
       </c>
@@ -2790,7 +3911,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>20</v>
       </c>
@@ -2798,7 +3919,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>20</v>
       </c>
@@ -2806,7 +3927,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>20</v>
       </c>
@@ -2814,7 +3935,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>20</v>
       </c>
@@ -2822,7 +3943,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>20</v>
       </c>
@@ -2830,7 +3951,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>20</v>
       </c>
@@ -2838,7 +3959,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>20</v>
       </c>
@@ -2846,7 +3967,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>20</v>
       </c>
@@ -2854,7 +3975,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>20</v>
       </c>
@@ -2862,7 +3983,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>0</v>
       </c>
@@ -2870,7 +3991,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>0</v>
       </c>
@@ -2878,7 +3999,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>0</v>
       </c>
@@ -2886,7 +4007,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>0</v>
       </c>
@@ -2894,7 +4015,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>0</v>
       </c>
@@ -2902,7 +4023,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>0</v>
       </c>
@@ -2910,7 +4031,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>0</v>
       </c>
@@ -2918,7 +4039,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>0</v>
       </c>
@@ -2926,7 +4047,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>0</v>
       </c>
@@ -2934,7 +4055,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>-20</v>
       </c>
@@ -2942,7 +4063,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>-20</v>
       </c>
@@ -2950,7 +4071,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>-20</v>
       </c>
@@ -2958,7 +4079,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>-20</v>
       </c>
@@ -2966,7 +4087,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>-20</v>
       </c>
@@ -2974,7 +4095,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>-20</v>
       </c>
@@ -2982,7 +4103,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>-20</v>
       </c>
@@ -2990,7 +4111,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>-20</v>
       </c>
@@ -2998,7 +4119,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>-20</v>
       </c>
@@ -3006,7 +4127,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>-50</v>
       </c>
@@ -3014,7 +4135,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>-50</v>
       </c>
@@ -3022,7 +4143,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>-50</v>
       </c>
@@ -3030,7 +4151,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>-50</v>
       </c>
@@ -3038,7 +4159,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>-50</v>
       </c>
@@ -3046,7 +4167,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>-50</v>
       </c>
@@ -3054,7 +4175,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>-80</v>
       </c>
@@ -3062,7 +4183,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>-80</v>
       </c>
@@ -3070,7 +4191,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>-80</v>
       </c>
@@ -3078,7 +4199,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>-80</v>
       </c>
@@ -3086,7 +4207,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>-80</v>
       </c>
@@ -3094,7 +4215,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>-80</v>
       </c>
@@ -3102,7 +4223,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>-80</v>
       </c>
@@ -3110,7 +4231,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>-80</v>
       </c>
@@ -3118,7 +4239,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>-80</v>
       </c>
@@ -3126,7 +4247,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>-195</v>
       </c>
@@ -3134,7 +4255,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>-195</v>
       </c>
@@ -3142,7 +4263,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>-195</v>
       </c>
@@ -3150,7 +4271,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>-195</v>
       </c>
@@ -3158,7 +4279,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>-195</v>
       </c>
@@ -3166,7 +4287,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>-195</v>
       </c>
@@ -3187,13 +4308,13 @@
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -3201,7 +4322,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>200</v>
       </c>
@@ -3209,7 +4330,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>200</v>
       </c>
@@ -3217,7 +4338,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>200</v>
       </c>
@@ -3225,7 +4346,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>200</v>
       </c>
@@ -3233,7 +4354,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>200</v>
       </c>
@@ -3241,7 +4362,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>200</v>
       </c>
@@ -3249,7 +4370,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>100</v>
       </c>
@@ -3257,7 +4378,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>100</v>
       </c>
@@ -3265,7 +4386,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>100</v>
       </c>
@@ -3273,7 +4394,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>100</v>
       </c>
@@ -3281,7 +4402,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>100</v>
       </c>
@@ -3289,7 +4410,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>100</v>
       </c>
@@ -3297,7 +4418,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>100</v>
       </c>
@@ -3305,7 +4426,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>100</v>
       </c>
@@ -3313,7 +4434,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>100</v>
       </c>
@@ -3321,7 +4442,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>80</v>
       </c>
@@ -3329,7 +4450,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>70</v>
       </c>
@@ -3337,7 +4458,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>50</v>
       </c>
@@ -3345,7 +4466,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>50</v>
       </c>
@@ -3353,7 +4474,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>50</v>
       </c>
@@ -3361,7 +4482,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>50</v>
       </c>
@@ -3369,7 +4490,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>50</v>
       </c>
@@ -3377,7 +4498,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>50</v>
       </c>
@@ -3385,7 +4506,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>20</v>
       </c>
@@ -3393,7 +4514,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>20</v>
       </c>
@@ -3401,7 +4522,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>20</v>
       </c>
@@ -3409,7 +4530,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>20</v>
       </c>
@@ -3417,7 +4538,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>20</v>
       </c>
@@ -3425,7 +4546,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>20</v>
       </c>
@@ -3433,7 +4554,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>20</v>
       </c>
@@ -3441,7 +4562,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>20</v>
       </c>
@@ -3449,7 +4570,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>-20</v>
       </c>
@@ -3457,7 +4578,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>-20</v>
       </c>
@@ -3465,7 +4586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>-20</v>
       </c>
@@ -3473,7 +4594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>-20</v>
       </c>
@@ -3481,7 +4602,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>-20</v>
       </c>
@@ -3489,7 +4610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>-20</v>
       </c>
@@ -3497,7 +4618,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>-20</v>
       </c>
@@ -3505,7 +4626,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>-20</v>
       </c>
@@ -3513,7 +4634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>-50</v>
       </c>
@@ -3521,7 +4642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>-50</v>
       </c>
@@ -3529,7 +4650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>-50</v>
       </c>
@@ -3537,7 +4658,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>-50</v>
       </c>
@@ -3545,7 +4666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>-50</v>
       </c>
@@ -3553,7 +4674,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>-50</v>
       </c>
@@ -3561,7 +4682,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>-50</v>
       </c>
@@ -3569,7 +4690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>-50</v>
       </c>
@@ -3577,7 +4698,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>-80</v>
       </c>
@@ -3585,7 +4706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>-80</v>
       </c>
@@ -3593,7 +4714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>-80</v>
       </c>
@@ -3601,7 +4722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>-80</v>
       </c>
@@ -3609,7 +4730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>-80</v>
       </c>
@@ -3617,7 +4738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>-80</v>
       </c>
@@ -3625,7 +4746,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>-80</v>
       </c>
@@ -3633,7 +4754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>-195</v>
       </c>
@@ -3641,7 +4762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>-195</v>
       </c>
@@ -3649,7 +4770,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>-195</v>
       </c>
@@ -3657,7 +4778,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>-195</v>
       </c>
@@ -3665,7 +4786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>-195</v>
       </c>
@@ -3673,7 +4794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>-195</v>
       </c>

</xml_diff>

<commit_message>
updated to include constrcution lines
</commit_message>
<xml_diff>
--- a/Lab work/Materials lab/Charpy and Hardness Data 2025.xlsx
+++ b/Lab work/Materials lab/Charpy and Hardness Data 2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/eb1723_ic_ac_uk/Documents/ME2/University computing/Lab work/Materials lab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="8_{1539A9E4-AFA8-425B-AFF2-01C484C56F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0A08DE6-8025-214D-B9D8-DEC4E32BAA36}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="8_{1539A9E4-AFA8-425B-AFF2-01C484C56F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE77A72B-3FEE-7448-AAB2-A49132A510F8}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{81260FE9-10E2-42F8-90B5-15DA67BC97B4}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16580" xr2:uid="{81260FE9-10E2-42F8-90B5-15DA67BC97B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hardness Data" sheetId="6" r:id="rId1"/>
@@ -27,10 +27,6 @@
     <definedName name="_xlchart.v1.3" hidden="1">'Hardness Data'!$V$3:$V$5</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">'Hardness Data'!$AA$3:$AA$5</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">'Hardness Data'!$V$3:$V$5</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'Hardness Data'!$AA$3:$AA$5</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'Hardness Data'!$V$3:$V$5</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'Hardness Data'!$AA$3:$AA$5</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'Hardness Data'!$V$3:$V$5</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -270,10 +266,8 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -293,6 +287,20 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
               <c:f>'Hardness Data'!$AA$3:$AA$5</c:f>
@@ -1562,7 +1570,7 @@
   <dimension ref="A2:AA16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="P1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AA24" sqref="AA24"/>
+      <selection activeCell="Z29" sqref="Z29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1786,26 +1794,26 @@
         <v>118.3</v>
       </c>
       <c r="V4" s="4">
-        <f t="shared" ref="V4:V5" si="0">SUM(B4:U4)/20</f>
+        <f t="shared" ref="V4" si="0">SUM(B4:U4)/20</f>
         <v>121.66500000000003</v>
       </c>
       <c r="W4" s="4">
-        <f t="shared" ref="W4:W5" si="1">MAX(B4:U4)</f>
+        <f t="shared" ref="W4" si="1">MAX(B4:U4)</f>
         <v>128.69999999999999</v>
       </c>
       <c r="X4" s="4">
-        <f t="shared" ref="X4:X5" si="2">MIN(B4:U4)</f>
+        <f t="shared" ref="X4" si="2">MIN(B4:U4)</f>
         <v>116.4</v>
       </c>
       <c r="Y4">
-        <f t="shared" ref="Y4:Y5" si="3">(W4-X4)/19</f>
+        <f t="shared" ref="Y4" si="3">(W4-X4)/19</f>
         <v>0.6473684210526307</v>
       </c>
       <c r="Z4">
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="AA4">
-        <f t="shared" ref="AA4:AA5" si="4">1/SQRT(Z4)</f>
+        <f t="shared" ref="AA4" si="4">1/SQRT(Z4)</f>
         <v>5.5901699437494745</v>
       </c>
     </row>

</xml_diff>